<commit_message>
feat(ui): add pause screen overlay and ESC toggle state
</commit_message>
<xml_diff>
--- a/design_src/MechParts.xlsx
+++ b/design_src/MechParts.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\000 move\Projects\TDFM\mech-td-prototype\design_src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63CD7B55-37A4-4A6F-95BE-E5DF6F5E2DAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25A8925B-DC8C-4AE0-9823-AC649EBDBEB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12030" yWindow="-11595" windowWidth="14400" windowHeight="8175" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12165" yWindow="-10215" windowWidth="14970" windowHeight="8175" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Body" sheetId="1" r:id="rId1"/>
-    <sheet name="Arm" sheetId="2" r:id="rId2"/>
-    <sheet name="Legs" sheetId="3" r:id="rId3"/>
+    <sheet name="#説明" sheetId="4" r:id="rId1"/>
+    <sheet name="Body" sheetId="1" r:id="rId2"/>
+    <sheet name="Arm" sheetId="2" r:id="rId3"/>
+    <sheet name="Legs" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="41">
   <si>
     <t>ID</t>
   </si>
@@ -38,9 +39,6 @@
     <t>Weight</t>
   </si>
   <si>
-    <t>Engine</t>
-  </si>
-  <si>
     <t>Defense</t>
   </si>
   <si>
@@ -89,24 +87,6 @@
     <t>Arm D</t>
   </si>
   <si>
-    <t>Accuracy</t>
-  </si>
-  <si>
-    <t>命中値</t>
-  </si>
-  <si>
-    <t>Legs A</t>
-  </si>
-  <si>
-    <t>Legs B</t>
-  </si>
-  <si>
-    <t>Legs C</t>
-  </si>
-  <si>
-    <t>Legs D</t>
-  </si>
-  <si>
     <t>種類</t>
   </si>
   <si>
@@ -116,20 +96,68 @@
     <t>normal</t>
   </si>
   <si>
-    <t>移動力</t>
-  </si>
-  <si>
-    <t>Movement</t>
-  </si>
-  <si>
     <t>uint</t>
+  </si>
+  <si>
+    <t>hover</t>
+  </si>
+  <si>
+    <t>機体は「胴」「腕（左）」「腕（右）」「両脚」の各部位で構成される。</t>
+  </si>
+  <si>
+    <t>概要</t>
+  </si>
+  <si>
+    <t>移動力補正</t>
+  </si>
+  <si>
+    <t>MovementSpeedMod</t>
+  </si>
+  <si>
+    <t>PowerOutput</t>
+  </si>
+  <si>
+    <t>AccuracyRatio</t>
+  </si>
+  <si>
+    <t>命中率</t>
+  </si>
+  <si>
+    <t>Regular</t>
+  </si>
+  <si>
+    <t>Legs A (Bipedal)</t>
+  </si>
+  <si>
+    <t>Higher Speed</t>
+  </si>
+  <si>
+    <t>Slow/Hover</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>#メモ</t>
+  </si>
+  <si>
+    <t>Legs D ()</t>
+  </si>
+  <si>
+    <t>High Speed</t>
+  </si>
+  <si>
+    <t>Legs B (Caterpillar)</t>
+  </si>
+  <si>
+    <t>Legs C (Hover)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -150,8 +178,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -161,6 +197,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -177,10 +219,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -460,153 +504,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B3E37EE-27A4-4BA1-BDCD-B7F970C79496}">
+  <dimension ref="B1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="3" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>11001</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4">
-        <v>8</v>
-      </c>
-      <c r="D4">
+    <row r="1" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B1" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
         <v>24</v>
-      </c>
-      <c r="E4">
-        <v>55</v>
-      </c>
-      <c r="F4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5">
-        <v>11002</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5">
-        <v>10</v>
-      </c>
-      <c r="D5">
-        <v>27</v>
-      </c>
-      <c r="E5">
-        <v>110</v>
-      </c>
-      <c r="F5">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6">
-        <v>11003</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6">
-        <v>11</v>
-      </c>
-      <c r="D6">
-        <v>33</v>
-      </c>
-      <c r="E6">
-        <v>130</v>
-      </c>
-      <c r="F6">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7">
-        <v>11004</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7">
-        <v>11</v>
-      </c>
-      <c r="D7">
-        <v>30</v>
-      </c>
-      <c r="E7">
-        <v>140</v>
-      </c>
-      <c r="F7">
-        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -616,152 +533,336 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{357834BD-C019-4247-80D6-8C22455E372D}">
-  <dimension ref="A1:F7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="20" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>11001</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4">
+        <v>8</v>
+      </c>
+      <c r="E4">
+        <v>24</v>
+      </c>
+      <c r="F4">
+        <v>55</v>
+      </c>
+      <c r="G4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>11002</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5">
+        <v>10</v>
+      </c>
+      <c r="E5">
+        <v>27</v>
+      </c>
+      <c r="F5">
+        <v>110</v>
+      </c>
+      <c r="G5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>11003</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6">
+        <v>11</v>
+      </c>
+      <c r="E6">
+        <v>33</v>
+      </c>
+      <c r="F6">
+        <v>130</v>
+      </c>
+      <c r="G6">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>11004</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7">
+        <v>11</v>
+      </c>
+      <c r="E7">
+        <v>30</v>
+      </c>
+      <c r="F7">
+        <v>140</v>
+      </c>
+      <c r="G7">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{357834BD-C019-4247-80D6-8C22455E372D}">
+  <dimension ref="A1:G7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="20" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>4</v>
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>35</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="F2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>31</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="C3" s="4"/>
       <c r="D3" s="1" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+        <v>22</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>12001</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4">
+        <v>15</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4">
         <v>9</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>19</v>
       </c>
-      <c r="E4">
-        <v>45</v>
-      </c>
       <c r="F4">
+        <v>8500</v>
+      </c>
+      <c r="G4">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>12002</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5">
+        <v>16</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5">
         <v>12</v>
       </c>
-      <c r="D5">
-        <v>22</v>
-      </c>
       <c r="E5">
-        <v>57</v>
+        <v>22</v>
       </c>
       <c r="F5">
+        <v>8800</v>
+      </c>
+      <c r="G5">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>12003</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6">
+        <v>14</v>
+      </c>
+      <c r="E6">
+        <v>24</v>
+      </c>
+      <c r="F6">
+        <v>9000</v>
+      </c>
+      <c r="G6">
         <v>18</v>
       </c>
-      <c r="C6">
-        <v>14</v>
-      </c>
-      <c r="D6">
-        <v>24</v>
-      </c>
-      <c r="E6">
-        <v>60</v>
-      </c>
-      <c r="F6">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>12004</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7">
+        <v>18</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7">
         <v>15</v>
       </c>
-      <c r="D7">
-        <v>22</v>
-      </c>
       <c r="E7">
-        <v>62</v>
+        <v>22</v>
       </c>
       <c r="F7">
+        <v>9200</v>
+      </c>
+      <c r="G7">
         <v>16</v>
       </c>
     </row>
@@ -770,136 +871,220 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89F5171B-255B-41AA-9F19-197956663F2E}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="3" width="20" customWidth="1"/>
+    <col min="6" max="6" width="13.08984375" customWidth="1"/>
+    <col min="7" max="7" width="12.81640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F3" s="1" t="s">
+      <c r="H3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>13001</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4">
+        <v>9</v>
+      </c>
+      <c r="E4">
+        <v>21</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>13</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>13002</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5">
+        <v>10</v>
+      </c>
+      <c r="E5">
+        <v>24</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>1500</v>
+      </c>
+      <c r="H5">
+        <v>18</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>13003</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+        <v>40</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6">
+        <v>13</v>
+      </c>
+      <c r="E6">
+        <v>26</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>-2000</v>
+      </c>
+      <c r="H6">
+        <v>20</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>13004</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>28</v>
+        <v>37</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7">
+        <v>14</v>
+      </c>
+      <c r="E7">
+        <v>24</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>3500</v>
+      </c>
+      <c r="H7">
+        <v>18</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>